<commit_message>
folding paper done + start 1D bush fire
</commit_message>
<xml_diff>
--- a/codingame_scraper/easy_20250202.xlsx
+++ b/codingame_scraper/easy_20250202.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\OneDrive\Documents\Programmation\codingame_py\codingame_scraper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/codingame_py/codingame_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DFC599-7965-42E8-AD64-7A7C32B56484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{76DFC599-7965-42E8-AD64-7A7C32B56484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5035449-70E3-4817-9AAE-6D32B80EFA20}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{DAF74345-0394-4152-BAE3-49A48D9F91A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="277">
   <si>
     <t>titre</t>
   </si>
@@ -870,7 +870,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1352,7 +1352,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1407,7 +1407,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1772,7 +1772,7 @@
   <dimension ref="A1:C274"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2272,6 +2272,9 @@
       </c>
       <c r="B45" s="1">
         <v>2972</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
offset_arrays done. start pikapcha
</commit_message>
<xml_diff>
--- a/codingame_scraper/easy_20250202.xlsx
+++ b/codingame_scraper/easy_20250202.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/codingame_py/codingame_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{76DFC599-7965-42E8-AD64-7A7C32B56484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5035449-70E3-4817-9AAE-6D32B80EFA20}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{76DFC599-7965-42E8-AD64-7A7C32B56484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C99EED1F-9A8B-47DA-A659-C87E1873C2D8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{DAF74345-0394-4152-BAE3-49A48D9F91A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="277">
   <si>
     <t>titre</t>
   </si>
@@ -1425,6 +1425,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DonnéesExternes_1" connectionId="1" xr16:uid="{A956B59B-E1C8-4AAA-93E2-E89F48FA74D7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
@@ -1771,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D60BEC-0E06-4BD5-B141-9F92C33BF3EF}">
   <dimension ref="A1:C274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2306,6 +2310,9 @@
       <c r="B48" s="1">
         <v>2928</v>
       </c>
+      <c r="C48" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
@@ -2313,6 +2320,9 @@
       </c>
       <c r="B49" s="1">
         <v>2772</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
license plate done, start bulk email
</commit_message>
<xml_diff>
--- a/codingame_scraper/easy_20250202.xlsx
+++ b/codingame_scraper/easy_20250202.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/codingame_py/codingame_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{76DFC599-7965-42E8-AD64-7A7C32B56484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C99EED1F-9A8B-47DA-A659-C87E1873C2D8}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{76DFC599-7965-42E8-AD64-7A7C32B56484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9C82D9F-6BD3-49C6-B7DF-409A53901E18}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{DAF74345-0394-4152-BAE3-49A48D9F91A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="277">
   <si>
     <t>titre</t>
   </si>
@@ -1776,7 +1776,7 @@
   <dimension ref="A1:C274"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2343,6 +2343,9 @@
       <c r="B51" s="1">
         <v>2626</v>
       </c>
+      <c r="C51" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -2373,6 +2376,9 @@
       <c r="B54" s="1">
         <v>2432</v>
       </c>
+      <c r="C54" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
@@ -2392,6 +2398,9 @@
       <c r="B56" s="1">
         <v>2408</v>
       </c>
+      <c r="C56" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
@@ -2410,6 +2419,9 @@
       </c>
       <c r="B58" s="1">
         <v>2318</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
abcde doen -star medium/gravity
</commit_message>
<xml_diff>
--- a/codingame_scraper/easy_20250202.xlsx
+++ b/codingame_scraper/easy_20250202.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/codingame_py/codingame_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{76DFC599-7965-42E8-AD64-7A7C32B56484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72DB4ACB-FD29-4649-8B73-E66D23535C23}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{76DFC599-7965-42E8-AD64-7A7C32B56484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45B3A094-143A-4965-8C7C-E0557CA0824D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{DAF74345-0394-4152-BAE3-49A48D9F91A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="277">
   <si>
     <t>titre</t>
   </si>
@@ -1425,10 +1425,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DonnéesExternes_1" connectionId="1" xr16:uid="{A956B59B-E1C8-4AAA-93E2-E89F48FA74D7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4" unboundColumnsRight="1">
@@ -1776,7 +1772,7 @@
   <dimension ref="A1:C274"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2519,6 +2515,9 @@
       <c r="B67" s="1">
         <v>1948</v>
       </c>
+      <c r="C67" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
@@ -2526,6 +2525,9 @@
       </c>
       <c r="B68" s="1">
         <v>1935</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
self driving car DONE
</commit_message>
<xml_diff>
--- a/codingame_scraper/easy_20250202.xlsx
+++ b/codingame_scraper/easy_20250202.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/codingame_py/codingame_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{76DFC599-7965-42E8-AD64-7A7C32B56484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8BDA3F4-ED29-4E70-9B7C-8D1ED09E3AE7}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{76DFC599-7965-42E8-AD64-7A7C32B56484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1A53644-E959-487C-A333-BA34AB25C11D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{DAF74345-0394-4152-BAE3-49A48D9F91A3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="277">
   <si>
     <t>titre</t>
   </si>
@@ -1776,7 +1776,7 @@
   <dimension ref="A1:C274"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2585,6 +2585,9 @@
       <c r="B73" s="1">
         <v>1890</v>
       </c>
+      <c r="C73" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
@@ -2592,6 +2595,9 @@
       </c>
       <c r="B74" s="1">
         <v>1886</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>